<commit_message>
Fixed the speed and pwm grapsh to put PWM on the x-axis
</commit_message>
<xml_diff>
--- a/Lab1/lab1Results.xlsx
+++ b/Lab1/lab1Results.xlsx
@@ -890,184 +890,188 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1364,8 +1368,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="30229348"/>
-        <c:axId val="81210010"/>
+        <c:axId val="61485303"/>
+        <c:axId val="97403365"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1548,11 +1552,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18257864"/>
-        <c:axId val="89023874"/>
+        <c:axId val="96659038"/>
+        <c:axId val="66225298"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30229348"/>
+        <c:axId val="61485303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,12 +1632,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81210010"/>
+        <c:crossAx val="97403365"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81210010"/>
+        <c:axId val="97403365"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,12 +1713,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30229348"/>
+        <c:crossAx val="61485303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18257864"/>
+        <c:axId val="96659038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,11 +1750,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89023874"/>
+        <c:crossAx val="66225298"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89023874"/>
+        <c:axId val="66225298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1820,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18257864"/>
+        <c:crossAx val="96659038"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,8 +2070,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="98801779"/>
-        <c:axId val="39245457"/>
+        <c:axId val="18331283"/>
+        <c:axId val="47517182"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2226,11 +2230,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="68112974"/>
-        <c:axId val="67247752"/>
+        <c:axId val="95324960"/>
+        <c:axId val="42435816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98801779"/>
+        <c:axId val="18331283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,12 +2310,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39245457"/>
+        <c:crossAx val="47517182"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39245457"/>
+        <c:axId val="47517182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,12 +2391,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98801779"/>
+        <c:crossAx val="18331283"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68112974"/>
+        <c:axId val="95324960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,11 +2428,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67247752"/>
+        <c:crossAx val="42435816"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67247752"/>
+        <c:axId val="42435816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2494,7 +2498,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68112974"/>
+        <c:crossAx val="95324960"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2769,8 +2773,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89161793"/>
-        <c:axId val="19721902"/>
+        <c:axId val="52434138"/>
+        <c:axId val="51040387"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2953,11 +2957,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="10296841"/>
-        <c:axId val="33527245"/>
+        <c:axId val="52373319"/>
+        <c:axId val="14943033"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89161793"/>
+        <c:axId val="52434138"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,12 +3037,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19721902"/>
+        <c:crossAx val="51040387"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19721902"/>
+        <c:axId val="51040387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3114,12 +3118,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89161793"/>
+        <c:crossAx val="52434138"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10296841"/>
+        <c:axId val="52373319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3151,11 +3155,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33527245"/>
+        <c:crossAx val="14943033"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33527245"/>
+        <c:axId val="14943033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3221,7 +3225,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10296841"/>
+        <c:crossAx val="52373319"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3472,8 +3476,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="62990220"/>
-        <c:axId val="35781983"/>
+        <c:axId val="97674353"/>
+        <c:axId val="91657236"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3656,11 +3660,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="39250685"/>
-        <c:axId val="8008267"/>
+        <c:axId val="18722890"/>
+        <c:axId val="27758769"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62990220"/>
+        <c:axId val="97674353"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,12 +3740,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35781983"/>
+        <c:crossAx val="91657236"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35781983"/>
+        <c:axId val="91657236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3817,12 +3821,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62990220"/>
+        <c:crossAx val="97674353"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39250685"/>
+        <c:axId val="18722890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,11 +3858,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8008267"/>
+        <c:crossAx val="27758769"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8008267"/>
+        <c:axId val="27758769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3924,7 +3928,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39250685"/>
+        <c:crossAx val="18722890"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4003,7 +4007,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>PWM vs Speed Motor A</a:t>
+              <a:t>Speed vs PWM Motor A</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4100,6 +4104,30 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet1!$S$9:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$U$9:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
@@ -4121,41 +4149,17 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$S$9:$S$13</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47251779"/>
-        <c:axId val="95182191"/>
+        <c:axId val="34948244"/>
+        <c:axId val="58832852"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47251779"/>
+        <c:axId val="34948244"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="90"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4173,6 +4177,88 @@
           <c:tx>
             <c:rich>
               <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>PWM (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58832852"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="58832852"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4229,89 +4315,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95182191"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="95182191"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>PWM (%)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="47251779"/>
+        <c:crossAx val="34948244"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4360,7 +4364,6 @@
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -4390,7 +4393,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>PWM vs Speed Motor B</a:t>
+              <a:t>Speed vs PWM Motor B</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4487,6 +4490,30 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet1!$S$26:$S$30</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$U$26:$U$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
@@ -4508,40 +4535,17 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$S$26:$S$30</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="23451717"/>
-        <c:axId val="5535070"/>
+        <c:axId val="99563074"/>
+        <c:axId val="35435526"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23451717"/>
+        <c:axId val="99563074"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4559,6 +4563,88 @@
           <c:tx>
             <c:rich>
               <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>PWM (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35435526"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="35435526"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4615,89 +4701,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5535070"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="5535070"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>PWM (%)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="23451717"/>
+        <c:crossAx val="99563074"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4761,9 +4765,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>87840</xdr:colOff>
+      <xdr:colOff>87480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4771,8 +4775,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21889800" y="2030400"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="21888720" y="2030400"/>
+        <a:ext cx="4995000" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4791,9 +4795,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4801,8 +4805,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21891960" y="5456160"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="21890880" y="5456160"/>
+        <a:ext cx="4995000" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4821,9 +4825,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>235080</xdr:colOff>
+      <xdr:colOff>234720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4831,8 +4835,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28152000" y="2079360"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="28150920" y="2079360"/>
+        <a:ext cx="4995360" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4851,9 +4855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>118800</xdr:colOff>
+      <xdr:colOff>118440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>120960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4861,8 +4865,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28035720" y="5262840"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="28034640" y="5262840"/>
+        <a:ext cx="4995360" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4881,9 +4885,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>43200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>178560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4891,8 +4895,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33464160" y="2091240"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="33463080" y="2091240"/>
+        <a:ext cx="4995000" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4911,18 +4915,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>76680</xdr:colOff>
+      <xdr:colOff>76320</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 6"/>
+        <xdr:cNvPr id="9" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33497280" y="5243040"/>
-        <a:ext cx="4995720" cy="2817000"/>
+        <a:off x="33496200" y="5243040"/>
+        <a:ext cx="4995000" cy="2816640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4943,8 +4947,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
+      <cdr:x>0.0719948111847795</cdr:x>
+      <cdr:y>0.127667731629393</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -4958,7 +4962,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
+          <a:ext cx="359640" cy="359640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4980,8 +4984,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
+      <cdr:x>0.0719948111847795</cdr:x>
+      <cdr:y>0.127667731629393</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -4995,7 +4999,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
+          <a:ext cx="359640" cy="359640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5017,8 +5021,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
+      <cdr:x>0.0719896231173885</cdr:x>
+      <cdr:y>0.127667731629393</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -5032,7 +5036,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
+          <a:ext cx="359640" cy="359640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5054,8 +5058,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
+      <cdr:x>0.0719896231173885</cdr:x>
+      <cdr:y>0.127667731629393</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -5069,7 +5073,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
+          <a:ext cx="359640" cy="359640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5091,12 +5095,12 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
+      <cdr:x>0.0719948111847795</cdr:x>
+      <cdr:y>0.127667731629393</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
-        <cdr:cNvPr id="9" name="" descr=""/>
+        <cdr:cNvPr id="10" name="" descr=""/>
         <cdr:cNvPicPr/>
       </cdr:nvPicPr>
       <cdr:blipFill>
@@ -5106,44 +5110,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </cdr:spPr>
-    </cdr:pic>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <cdr:relSizeAnchor>
-    <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.0720564922899553</cdr:x>
-      <cdr:y>0.127779197546639</cdr:y>
-    </cdr:to>
-    <cdr:pic>
-      <cdr:nvPicPr>
-        <cdr:cNvPr id="11" name="" descr=""/>
-        <cdr:cNvPicPr/>
-      </cdr:nvPicPr>
-      <cdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </cdr:blipFill>
-      <cdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
+          <a:ext cx="359640" cy="359640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5336,1821 +5303,1821 @@
   </sheetPr>
   <dimension ref="A1:AX36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V5" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO6" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BB27" activeCellId="0" sqref="BB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="1" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="11.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="16.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="P4" s="2" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="P4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3"/>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="4"/>
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="S7" s="6" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="S7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="W7" s="6" t="s">
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="W7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="X7" s="6"/>
+      <c r="X7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="4"/>
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="10" t="s">
+      <c r="T8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="U8" s="11" t="s">
+      <c r="U8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="11" t="s">
+      <c r="X8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AK8" s="12" t="s">
+      <c r="AK8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AL8" s="12"/>
-      <c r="AM8" s="12"/>
-      <c r="AN8" s="12"/>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="12"/>
-      <c r="AS8" s="12" t="s">
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AS8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AT8" s="12"/>
-      <c r="AU8" s="12"/>
-      <c r="AV8" s="12"/>
-      <c r="AW8" s="12"/>
-      <c r="AX8" s="12"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+      <c r="AX8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="14" t="n">
+      <c r="F9" s="15" t="n">
         <v>3.486</v>
       </c>
-      <c r="G9" s="13" t="n">
+      <c r="G9" s="14" t="n">
         <v>92.86</v>
       </c>
-      <c r="H9" s="15" t="n">
+      <c r="H9" s="16" t="n">
         <v>4.06</v>
       </c>
-      <c r="I9" s="16" t="n">
+      <c r="I9" s="17" t="n">
         <f aca="false">$C$12/F9</f>
         <v>0.16924842226047</v>
       </c>
-      <c r="J9" s="16" t="n">
+      <c r="J9" s="17" t="n">
         <f aca="false">I9/$C$11</f>
         <v>9.02658252055842</v>
       </c>
-      <c r="K9" s="17" t="n">
+      <c r="K9" s="18" t="n">
         <f aca="false">J9*(1/(2*PI()))*60</f>
         <v>86.1975136424264</v>
       </c>
-      <c r="L9" s="18" t="n">
+      <c r="L9" s="19" t="n">
         <f aca="false">E9*$C$13</f>
         <v>0</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="M9" s="12" t="n">
         <f aca="false">L9*9.81</f>
         <v>0</v>
       </c>
-      <c r="N9" s="11" t="n">
+      <c r="N9" s="12" t="n">
         <f aca="false">M9*$C$11*1000</f>
         <v>0</v>
       </c>
-      <c r="O9" s="19" t="n">
+      <c r="O9" s="20" t="n">
         <f aca="false">H9*G9</f>
         <v>377.0116</v>
       </c>
-      <c r="P9" s="17" t="n">
+      <c r="P9" s="18" t="n">
         <f aca="false">J9*N9</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="10" t="n">
+      <c r="Q9" s="11" t="n">
         <f aca="false">P9/O9*100</f>
         <v>0</v>
       </c>
-      <c r="S9" s="20" t="n">
+      <c r="S9" s="21" t="n">
         <v>20</v>
       </c>
-      <c r="T9" s="21" t="n">
+      <c r="T9" s="22" t="n">
         <v>54.956</v>
       </c>
-      <c r="U9" s="11" t="n">
+      <c r="U9" s="12" t="n">
         <f aca="false">($C$12/T9)*(1/$C$11)*(1/(2*PI()))*60</f>
         <v>5.46772932086575</v>
       </c>
-      <c r="W9" s="22" t="n">
+      <c r="W9" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="X9" s="15" t="n">
+      <c r="X9" s="16" t="n">
         <v>6.763</v>
       </c>
-      <c r="AK9" s="12"/>
-      <c r="AL9" s="12"/>
-      <c r="AM9" s="12"/>
-      <c r="AN9" s="12"/>
-      <c r="AO9" s="12"/>
-      <c r="AP9" s="12"/>
-      <c r="AS9" s="12"/>
-      <c r="AT9" s="12"/>
-      <c r="AU9" s="12"/>
-      <c r="AV9" s="12"/>
-      <c r="AW9" s="12"/>
-      <c r="AX9" s="12"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+      <c r="AX9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="E10" s="13" t="n">
+      <c r="C10" s="6"/>
+      <c r="E10" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="14" t="n">
+      <c r="F10" s="15" t="n">
         <v>3.879</v>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="14" t="n">
         <v>92.38</v>
       </c>
-      <c r="H10" s="23" t="n">
+      <c r="H10" s="24" t="n">
         <v>4.05</v>
       </c>
-      <c r="I10" s="16" t="n">
+      <c r="I10" s="17" t="n">
         <f aca="false">$C$12/F10</f>
         <v>0.152101056973447</v>
       </c>
-      <c r="J10" s="16" t="n">
+      <c r="J10" s="17" t="n">
         <f aca="false">I10/$C$11</f>
         <v>8.11205637191716</v>
       </c>
-      <c r="K10" s="17" t="n">
+      <c r="K10" s="18" t="n">
         <f aca="false">J10*(1/(2*PI()))*60</f>
         <v>77.4644322138434</v>
       </c>
-      <c r="L10" s="18" t="n">
+      <c r="L10" s="19" t="n">
         <f aca="false">E10*$C$13</f>
         <v>0.042</v>
       </c>
-      <c r="M10" s="16" t="n">
+      <c r="M10" s="17" t="n">
         <f aca="false">L10*9.81</f>
         <v>0.41202</v>
       </c>
-      <c r="N10" s="16" t="n">
+      <c r="N10" s="17" t="n">
         <f aca="false">M10*$C$11*1000</f>
         <v>7.725375</v>
       </c>
-      <c r="O10" s="19" t="n">
+      <c r="O10" s="20" t="n">
         <f aca="false">H10*G10</f>
         <v>374.139</v>
       </c>
-      <c r="P10" s="17" t="n">
+      <c r="P10" s="18" t="n">
         <f aca="false">J10*N10</f>
         <v>62.6686774941995</v>
       </c>
-      <c r="Q10" s="10" t="n">
+      <c r="Q10" s="11" t="n">
         <f aca="false">P10/O10*100</f>
         <v>16.7501055741849</v>
       </c>
-      <c r="S10" s="24" t="n">
+      <c r="S10" s="25" t="n">
         <v>40</v>
       </c>
-      <c r="T10" s="25" t="n">
+      <c r="T10" s="26" t="n">
         <v>11.531</v>
       </c>
-      <c r="U10" s="16" t="n">
+      <c r="U10" s="17" t="n">
         <f aca="false">($C$12/T10)*(1/$C$11)*(1/(2*PI()))*60</f>
         <v>26.0588442075708</v>
       </c>
-      <c r="W10" s="9" t="n">
+      <c r="W10" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="X10" s="23" t="n">
+      <c r="X10" s="24" t="n">
         <v>6.81</v>
       </c>
-      <c r="AK10" s="12"/>
-      <c r="AL10" s="12"/>
-      <c r="AM10" s="12"/>
-      <c r="AN10" s="12"/>
-      <c r="AO10" s="12"/>
-      <c r="AP10" s="12"/>
-      <c r="AS10" s="12"/>
-      <c r="AT10" s="12"/>
-      <c r="AU10" s="12"/>
-      <c r="AV10" s="12"/>
-      <c r="AW10" s="12"/>
-      <c r="AX10" s="12"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+      <c r="AX10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="24" t="n">
         <v>0.01875</v>
       </c>
-      <c r="E11" s="13" t="n">
+      <c r="E11" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="14" t="n">
+      <c r="F11" s="15" t="n">
         <v>4.179</v>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G11" s="14" t="n">
         <v>107.53</v>
       </c>
-      <c r="H11" s="23" t="n">
+      <c r="H11" s="24" t="n">
         <v>3.9</v>
       </c>
-      <c r="I11" s="16" t="n">
+      <c r="I11" s="17" t="n">
         <f aca="false">$C$12/F11</f>
         <v>0.141182100981096</v>
       </c>
-      <c r="J11" s="16" t="n">
+      <c r="J11" s="17" t="n">
         <f aca="false">I11/$C$11</f>
         <v>7.52971205232512</v>
       </c>
-      <c r="K11" s="17" t="n">
+      <c r="K11" s="18" t="n">
         <f aca="false">J11*(1/(2*PI()))*60</f>
         <v>71.9034535911698</v>
       </c>
-      <c r="L11" s="18" t="n">
+      <c r="L11" s="19" t="n">
         <f aca="false">E11*$C$13</f>
         <v>0.084</v>
       </c>
-      <c r="M11" s="16" t="n">
+      <c r="M11" s="17" t="n">
         <f aca="false">L11*9.81</f>
         <v>0.82404</v>
       </c>
-      <c r="N11" s="16" t="n">
+      <c r="N11" s="17" t="n">
         <f aca="false">M11*$C$11*1000</f>
         <v>15.45075</v>
       </c>
-      <c r="O11" s="19" t="n">
+      <c r="O11" s="20" t="n">
         <f aca="false">H11*G11</f>
         <v>419.367</v>
       </c>
-      <c r="P11" s="17" t="n">
+      <c r="P11" s="18" t="n">
         <f aca="false">J11*N11</f>
         <v>116.339698492462</v>
       </c>
-      <c r="Q11" s="10" t="n">
+      <c r="Q11" s="11" t="n">
         <f aca="false">P11/O11*100</f>
         <v>27.7417389762338</v>
       </c>
-      <c r="S11" s="24" t="n">
+      <c r="S11" s="25" t="n">
         <v>60</v>
       </c>
-      <c r="T11" s="25" t="n">
+      <c r="T11" s="26" t="n">
         <v>7.54</v>
       </c>
-      <c r="U11" s="16" t="n">
+      <c r="U11" s="17" t="n">
         <f aca="false">($C$12/T11)*(1/$C$11)*(1/(2*PI()))*60</f>
         <v>39.8520600208884</v>
       </c>
-      <c r="W11" s="9" t="n">
+      <c r="W11" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="X11" s="23" t="n">
+      <c r="X11" s="24" t="n">
         <v>6.85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="24" t="n">
         <v>0.59</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E12" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="14" t="n">
+      <c r="F12" s="15" t="n">
         <v>4.593</v>
       </c>
-      <c r="G12" s="13" t="n">
+      <c r="G12" s="14" t="n">
         <v>125.12</v>
       </c>
-      <c r="H12" s="23" t="n">
+      <c r="H12" s="24" t="n">
         <v>3.71</v>
       </c>
-      <c r="I12" s="16" t="n">
+      <c r="I12" s="17" t="n">
         <f aca="false">$C$12/F12</f>
         <v>0.128456346614413</v>
       </c>
-      <c r="J12" s="16" t="n">
+      <c r="J12" s="17" t="n">
         <f aca="false">I12/$C$11</f>
         <v>6.85100515276871</v>
       </c>
-      <c r="K12" s="17" t="n">
+      <c r="K12" s="18" t="n">
         <f aca="false">J12*(1/(2*PI()))*60</f>
         <v>65.4222801126711</v>
       </c>
-      <c r="L12" s="18" t="n">
+      <c r="L12" s="19" t="n">
         <f aca="false">E12*$C$13</f>
         <v>0.126</v>
       </c>
-      <c r="M12" s="16" t="n">
+      <c r="M12" s="17" t="n">
         <f aca="false">L12*9.81</f>
         <v>1.23606</v>
       </c>
-      <c r="N12" s="16" t="n">
+      <c r="N12" s="17" t="n">
         <f aca="false">M12*$C$11*1000</f>
         <v>23.176125</v>
       </c>
-      <c r="O12" s="19" t="n">
+      <c r="O12" s="20" t="n">
         <f aca="false">H12*G12</f>
         <v>464.1952</v>
       </c>
-      <c r="P12" s="17" t="n">
+      <c r="P12" s="18" t="n">
         <f aca="false">J12*N12</f>
         <v>158.779751796212</v>
       </c>
-      <c r="Q12" s="10" t="n">
+      <c r="Q12" s="11" t="n">
         <f aca="false">P12/O12*100</f>
         <v>34.205384242709</v>
       </c>
-      <c r="S12" s="24" t="n">
+      <c r="S12" s="25" t="n">
         <v>80</v>
       </c>
-      <c r="T12" s="25" t="n">
+      <c r="T12" s="26" t="n">
         <v>6.245</v>
       </c>
-      <c r="U12" s="16" t="n">
+      <c r="U12" s="17" t="n">
         <f aca="false">($C$12/T12)*(1/$C$11)*(1/(2*PI()))*60</f>
         <v>48.1160180236186</v>
       </c>
-      <c r="W12" s="9" t="n">
+      <c r="W12" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="X12" s="23" t="n">
+      <c r="X12" s="24" t="n">
         <v>6.666</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="28" t="n">
+      <c r="C13" s="29" t="n">
         <v>0.042</v>
       </c>
-      <c r="E13" s="13" t="n">
+      <c r="E13" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="14" t="n">
+      <c r="F13" s="15" t="n">
         <v>5.151</v>
       </c>
-      <c r="G13" s="13" t="n">
+      <c r="G13" s="14" t="n">
         <v>176.93</v>
       </c>
-      <c r="H13" s="23" t="n">
+      <c r="H13" s="24" t="n">
         <v>3.19</v>
       </c>
-      <c r="I13" s="16" t="n">
+      <c r="I13" s="17" t="n">
         <f aca="false">$C$12/F13</f>
         <v>0.114540865851291</v>
       </c>
-      <c r="J13" s="16" t="n">
+      <c r="J13" s="17" t="n">
         <f aca="false">I13/$C$11</f>
         <v>6.10884617873552</v>
       </c>
-      <c r="K13" s="17" t="n">
+      <c r="K13" s="18" t="n">
         <f aca="false">J13*(1/(2*PI()))*60</f>
         <v>58.3351839560277</v>
       </c>
-      <c r="L13" s="18" t="n">
+      <c r="L13" s="19" t="n">
         <f aca="false">E13*$C$13</f>
         <v>0.168</v>
       </c>
-      <c r="M13" s="16" t="n">
+      <c r="M13" s="17" t="n">
         <f aca="false">L13*9.81</f>
         <v>1.64808</v>
       </c>
-      <c r="N13" s="16" t="n">
+      <c r="N13" s="17" t="n">
         <f aca="false">M13*$C$11*1000</f>
         <v>30.9015</v>
       </c>
-      <c r="O13" s="19" t="n">
+      <c r="O13" s="20" t="n">
         <f aca="false">H13*G13</f>
         <v>564.4067</v>
       </c>
-      <c r="P13" s="17" t="n">
+      <c r="P13" s="18" t="n">
         <f aca="false">J13*N13</f>
         <v>188.772510192196</v>
       </c>
-      <c r="Q13" s="10" t="n">
+      <c r="Q13" s="11" t="n">
         <f aca="false">P13/O13*100</f>
         <v>33.4461852051359</v>
       </c>
-      <c r="S13" s="29" t="n">
+      <c r="S13" s="30" t="n">
         <v>100</v>
       </c>
-      <c r="T13" s="30" t="n">
+      <c r="T13" s="31" t="n">
         <v>4.915</v>
       </c>
-      <c r="U13" s="31" t="n">
+      <c r="U13" s="32" t="n">
         <f aca="false">($C$12/T13)*(1/$C$11)*(1/(2*PI()))*60</f>
         <v>61.1362222904371</v>
       </c>
-      <c r="W13" s="9" t="n">
+      <c r="W13" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="X13" s="23" t="n">
+      <c r="X13" s="24" t="n">
         <v>6.876</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="13" t="n">
+      <c r="E14" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="14" t="n">
+      <c r="F14" s="15" t="n">
         <v>5.739</v>
       </c>
-      <c r="G14" s="13" t="n">
+      <c r="G14" s="14" t="n">
         <v>182.8</v>
       </c>
-      <c r="H14" s="23" t="n">
+      <c r="H14" s="24" t="n">
         <v>3.12</v>
       </c>
-      <c r="I14" s="16" t="n">
+      <c r="I14" s="17" t="n">
         <f aca="false">$C$12/F14</f>
         <v>0.102805366788639</v>
       </c>
-      <c r="J14" s="16" t="n">
+      <c r="J14" s="17" t="n">
         <f aca="false">I14/$C$11</f>
         <v>5.48295289539409</v>
       </c>
-      <c r="K14" s="17" t="n">
+      <c r="K14" s="18" t="n">
         <f aca="false">J14*(1/(2*PI()))*60</f>
         <v>52.3583433625193</v>
       </c>
-      <c r="L14" s="18" t="n">
+      <c r="L14" s="19" t="n">
         <f aca="false">E14*$C$13</f>
         <v>0.21</v>
       </c>
-      <c r="M14" s="16" t="n">
+      <c r="M14" s="17" t="n">
         <f aca="false">L14*9.81</f>
         <v>2.0601</v>
       </c>
-      <c r="N14" s="16" t="n">
+      <c r="N14" s="17" t="n">
         <f aca="false">M14*$C$11*1000</f>
         <v>38.626875</v>
       </c>
-      <c r="O14" s="19" t="n">
+      <c r="O14" s="20" t="n">
         <f aca="false">H14*G14</f>
         <v>570.336</v>
       </c>
-      <c r="P14" s="17" t="n">
+      <c r="P14" s="18" t="n">
         <f aca="false">J14*N14</f>
         <v>211.789336121276</v>
       </c>
-      <c r="Q14" s="10" t="n">
+      <c r="Q14" s="11" t="n">
         <f aca="false">P14/O14*100</f>
         <v>37.134134285978</v>
       </c>
-      <c r="W14" s="9" t="n">
+      <c r="W14" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="X14" s="23" t="n">
+      <c r="X14" s="24" t="n">
         <v>6.643</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="13" t="n">
+      <c r="E15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="14" t="n">
+      <c r="F15" s="15" t="n">
         <v>6.871</v>
       </c>
-      <c r="G15" s="13" t="n">
+      <c r="G15" s="14" t="n">
         <v>192.57</v>
       </c>
-      <c r="H15" s="23" t="n">
+      <c r="H15" s="24" t="n">
         <v>3.01</v>
       </c>
-      <c r="I15" s="16" t="n">
+      <c r="I15" s="17" t="n">
         <f aca="false">$C$12/F15</f>
         <v>0.0858681414641246</v>
       </c>
-      <c r="J15" s="16" t="n">
+      <c r="J15" s="17" t="n">
         <f aca="false">I15/$C$11</f>
         <v>4.57963421141998</v>
       </c>
-      <c r="K15" s="17" t="n">
+      <c r="K15" s="18" t="n">
         <f aca="false">J15*(1/(2*PI()))*60</f>
         <v>43.7322853380146</v>
       </c>
-      <c r="L15" s="18" t="n">
+      <c r="L15" s="19" t="n">
         <f aca="false">E15*$C$13</f>
         <v>0.252</v>
       </c>
-      <c r="M15" s="16" t="n">
+      <c r="M15" s="17" t="n">
         <f aca="false">L15*9.81</f>
         <v>2.47212</v>
       </c>
-      <c r="N15" s="16" t="n">
+      <c r="N15" s="17" t="n">
         <f aca="false">M15*$C$11*1000</f>
         <v>46.35225</v>
       </c>
-      <c r="O15" s="19" t="n">
+      <c r="O15" s="20" t="n">
         <f aca="false">H15*G15</f>
         <v>579.6357</v>
       </c>
-      <c r="P15" s="17" t="n">
+      <c r="P15" s="18" t="n">
         <f aca="false">J15*N15</f>
         <v>212.276349876292</v>
       </c>
-      <c r="Q15" s="10" t="n">
+      <c r="Q15" s="11" t="n">
         <f aca="false">P15/O15*100</f>
         <v>36.6223733072845</v>
       </c>
-      <c r="W15" s="9" t="n">
+      <c r="W15" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="X15" s="23" t="n">
+      <c r="X15" s="24" t="n">
         <v>6.876</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="13" t="n">
+      <c r="E16" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F16" s="14" t="n">
+      <c r="F16" s="15" t="n">
         <v>7.871</v>
       </c>
-      <c r="G16" s="13" t="n">
+      <c r="G16" s="14" t="n">
         <v>221.9</v>
       </c>
-      <c r="H16" s="23" t="n">
+      <c r="H16" s="24" t="n">
         <v>2.72</v>
       </c>
-      <c r="I16" s="16" t="n">
+      <c r="I16" s="17" t="n">
         <f aca="false">$C$12/F16</f>
         <v>0.0749587091856181</v>
       </c>
-      <c r="J16" s="16" t="n">
+      <c r="J16" s="17" t="n">
         <f aca="false">I16/$C$11</f>
         <v>3.99779782323296</v>
       </c>
-      <c r="K16" s="17" t="n">
+      <c r="K16" s="18" t="n">
         <f aca="false">J16*(1/(2*PI()))*60</f>
         <v>38.1761571029727</v>
       </c>
-      <c r="L16" s="18" t="n">
+      <c r="L16" s="19" t="n">
         <f aca="false">E16*$C$13</f>
         <v>0.294</v>
       </c>
-      <c r="M16" s="16" t="n">
+      <c r="M16" s="17" t="n">
         <f aca="false">L16*9.81</f>
         <v>2.88414</v>
       </c>
-      <c r="N16" s="16" t="n">
+      <c r="N16" s="17" t="n">
         <f aca="false">M16*$C$11*1000</f>
         <v>54.077625</v>
       </c>
-      <c r="O16" s="19" t="n">
+      <c r="O16" s="20" t="n">
         <f aca="false">H16*G16</f>
         <v>603.568</v>
       </c>
-      <c r="P16" s="17" t="n">
+      <c r="P16" s="18" t="n">
         <f aca="false">J16*N16</f>
         <v>216.191411510609</v>
       </c>
-      <c r="Q16" s="10" t="n">
+      <c r="Q16" s="11" t="n">
         <f aca="false">P16/O16*100</f>
         <v>35.8188988665086</v>
       </c>
-      <c r="W16" s="9" t="n">
+      <c r="W16" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="X16" s="23" t="n">
+      <c r="X16" s="24" t="n">
         <v>6.579</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E17" s="13" t="n">
+      <c r="E17" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F17" s="14" t="n">
+      <c r="F17" s="15" t="n">
         <v>9.537</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="14" t="n">
         <v>240.47</v>
       </c>
-      <c r="H17" s="23" t="n">
+      <c r="H17" s="24" t="n">
         <v>2.52</v>
       </c>
-      <c r="I17" s="16" t="n">
+      <c r="I17" s="17" t="n">
         <f aca="false">$C$12/F17</f>
         <v>0.0618643179196812</v>
       </c>
-      <c r="J17" s="16" t="n">
+      <c r="J17" s="17" t="n">
         <f aca="false">I17/$C$11</f>
         <v>3.29943028904967</v>
       </c>
-      <c r="K17" s="17" t="n">
+      <c r="K17" s="18" t="n">
         <f aca="false">J17*(1/(2*PI()))*60</f>
         <v>31.5072383933625</v>
       </c>
-      <c r="L17" s="18" t="n">
+      <c r="L17" s="19" t="n">
         <f aca="false">E17*$C$13</f>
         <v>0.336</v>
       </c>
-      <c r="M17" s="16" t="n">
+      <c r="M17" s="17" t="n">
         <f aca="false">L17*9.81</f>
         <v>3.29616</v>
       </c>
-      <c r="N17" s="16" t="n">
+      <c r="N17" s="17" t="n">
         <f aca="false">M17*$C$11*1000</f>
         <v>61.803</v>
       </c>
-      <c r="O17" s="19" t="n">
+      <c r="O17" s="20" t="n">
         <f aca="false">H17*G17</f>
         <v>605.9844</v>
       </c>
-      <c r="P17" s="17" t="n">
+      <c r="P17" s="18" t="n">
         <f aca="false">J17*N17</f>
         <v>203.914690154137</v>
       </c>
-      <c r="Q17" s="10" t="n">
+      <c r="Q17" s="11" t="n">
         <f aca="false">P17/O17*100</f>
         <v>33.650155045928</v>
       </c>
-      <c r="W17" s="9" t="n">
+      <c r="W17" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="X17" s="23" t="n">
+      <c r="X17" s="24" t="n">
         <v>6.694</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="F18" s="14" t="n">
+      <c r="F18" s="15" t="n">
         <v>11.148</v>
       </c>
-      <c r="G18" s="13" t="n">
+      <c r="G18" s="14" t="n">
         <v>281.52</v>
       </c>
-      <c r="H18" s="23" t="n">
+      <c r="H18" s="24" t="n">
         <v>2.1</v>
       </c>
-      <c r="I18" s="16" t="n">
+      <c r="I18" s="17" t="n">
         <f aca="false">$C$12/F18</f>
         <v>0.052924291352709</v>
       </c>
-      <c r="J18" s="16" t="n">
+      <c r="J18" s="17" t="n">
         <f aca="false">I18/$C$11</f>
         <v>2.82262887214448</v>
       </c>
-      <c r="K18" s="17" t="n">
+      <c r="K18" s="18" t="n">
         <f aca="false">J18*(1/(2*PI()))*60</f>
         <v>26.9541202509417</v>
       </c>
-      <c r="L18" s="18" t="n">
+      <c r="L18" s="19" t="n">
         <f aca="false">E18*$C$13</f>
         <v>0.378</v>
       </c>
-      <c r="M18" s="16" t="n">
+      <c r="M18" s="17" t="n">
         <f aca="false">L18*9.81</f>
         <v>3.70818</v>
       </c>
-      <c r="N18" s="16" t="n">
+      <c r="N18" s="17" t="n">
         <f aca="false">M18*$C$11*1000</f>
         <v>69.528375</v>
       </c>
-      <c r="O18" s="19" t="n">
+      <c r="O18" s="20" t="n">
         <f aca="false">H18*G18</f>
         <v>591.192</v>
       </c>
-      <c r="P18" s="17" t="n">
+      <c r="P18" s="18" t="n">
         <f aca="false">J18*N18</f>
         <v>196.252798708288</v>
       </c>
-      <c r="Q18" s="10" t="n">
+      <c r="Q18" s="11" t="n">
         <f aca="false">P18/O18*100</f>
         <v>33.1961188088283</v>
       </c>
-      <c r="W18" s="32" t="n">
+      <c r="W18" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="X18" s="28" t="n">
+      <c r="X18" s="29" t="n">
         <v>6.604</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="33" t="n">
+      <c r="E19" s="34" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="34" t="n">
+      <c r="F19" s="35" t="n">
         <v>13.703</v>
       </c>
-      <c r="G19" s="33" t="n">
+      <c r="G19" s="34" t="n">
         <v>304.5</v>
       </c>
-      <c r="H19" s="28" t="n">
+      <c r="H19" s="29" t="n">
         <v>1.87</v>
       </c>
-      <c r="I19" s="31" t="n">
+      <c r="I19" s="32" t="n">
         <f aca="false">$C$12/F19</f>
         <v>0.0430562650514486</v>
       </c>
-      <c r="J19" s="31" t="n">
+      <c r="J19" s="32" t="n">
         <f aca="false">I19/$C$11</f>
         <v>2.29633413607726</v>
       </c>
-      <c r="K19" s="35" t="n">
+      <c r="K19" s="36" t="n">
         <f aca="false">J19*(1/(2*PI()))*60</f>
         <v>21.9283757248412</v>
       </c>
-      <c r="L19" s="36" t="n">
+      <c r="L19" s="37" t="n">
         <f aca="false">E19*$C$13</f>
         <v>0.42</v>
       </c>
-      <c r="M19" s="31" t="n">
+      <c r="M19" s="32" t="n">
         <f aca="false">L19*9.81</f>
         <v>4.1202</v>
       </c>
-      <c r="N19" s="31" t="n">
+      <c r="N19" s="32" t="n">
         <f aca="false">M19*$C$11*1000</f>
         <v>77.25375</v>
       </c>
-      <c r="O19" s="35" t="n">
+      <c r="O19" s="36" t="n">
         <f aca="false">H19*G19</f>
         <v>569.415</v>
       </c>
-      <c r="P19" s="35" t="n">
+      <c r="P19" s="36" t="n">
         <f aca="false">J19*N19</f>
         <v>177.400423264978</v>
       </c>
-      <c r="Q19" s="37" t="n">
+      <c r="Q19" s="38" t="n">
         <f aca="false">P19/O19*100</f>
         <v>31.1548559951843</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="33" t="n">
+      <c r="E20" s="34" t="n">
         <v>11</v>
       </c>
-      <c r="F20" s="34" t="n">
+      <c r="F20" s="35" t="n">
         <v>19.253</v>
       </c>
-      <c r="G20" s="33" t="n">
+      <c r="G20" s="34" t="n">
         <v>338.71</v>
       </c>
-      <c r="H20" s="28" t="n">
+      <c r="H20" s="29" t="n">
         <v>1.53</v>
       </c>
-      <c r="I20" s="31" t="n">
+      <c r="I20" s="32" t="n">
         <f aca="false">$C$12/F20</f>
         <v>0.0306445748714486</v>
       </c>
-      <c r="J20" s="31" t="n">
+      <c r="J20" s="32" t="n">
         <f aca="false">I20/$C$11</f>
         <v>1.63437732647726</v>
       </c>
-      <c r="K20" s="35" t="n">
+      <c r="K20" s="36" t="n">
         <f aca="false">J20*(1/(2*PI()))*60</f>
         <v>15.6071538231703</v>
       </c>
-      <c r="L20" s="36" t="n">
+      <c r="L20" s="37" t="n">
         <f aca="false">E20*$C$13</f>
         <v>0.462</v>
       </c>
-      <c r="M20" s="31" t="n">
+      <c r="M20" s="32" t="n">
         <f aca="false">L20*9.81</f>
         <v>4.53222</v>
       </c>
-      <c r="N20" s="31" t="n">
+      <c r="N20" s="32" t="n">
         <f aca="false">M20*$C$11*1000</f>
         <v>84.979125</v>
       </c>
-      <c r="O20" s="35" t="n">
+      <c r="O20" s="36" t="n">
         <f aca="false">H20*G20</f>
         <v>518.2263</v>
       </c>
-      <c r="P20" s="35" t="n">
+      <c r="P20" s="36" t="n">
         <f aca="false">J20*N20</f>
         <v>138.887955123877</v>
       </c>
-      <c r="Q20" s="37" t="n">
+      <c r="Q20" s="38" t="n">
         <f aca="false">P20/O20*100</f>
         <v>26.800638084921</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="38" t="n">
+      <c r="E21" s="39" t="n">
         <v>12</v>
       </c>
-      <c r="F21" s="39" t="n">
+      <c r="F21" s="40" t="n">
         <v>34.88</v>
       </c>
-      <c r="G21" s="38" t="n">
+      <c r="G21" s="39" t="n">
         <v>318.18</v>
       </c>
-      <c r="H21" s="40" t="n">
+      <c r="H21" s="41" t="n">
         <v>1.72</v>
       </c>
-      <c r="I21" s="41" t="n">
+      <c r="I21" s="42" t="n">
         <f aca="false">$C$12/F21</f>
         <v>0.0169151376146789</v>
       </c>
-      <c r="J21" s="41" t="n">
+      <c r="J21" s="42" t="n">
         <f aca="false">I21/$C$11</f>
         <v>0.902140672782875</v>
       </c>
-      <c r="K21" s="42" t="n">
+      <c r="K21" s="43" t="n">
         <f aca="false">J21*(1/(2*PI()))*60</f>
         <v>8.61480884625856</v>
       </c>
-      <c r="L21" s="41" t="n">
+      <c r="L21" s="42" t="n">
         <f aca="false">E21*$C$13</f>
         <v>0.504</v>
       </c>
-      <c r="M21" s="41" t="n">
+      <c r="M21" s="42" t="n">
         <f aca="false">L21*9.81</f>
         <v>4.94424</v>
       </c>
-      <c r="N21" s="41" t="n">
+      <c r="N21" s="42" t="n">
         <f aca="false">M21*$C$11*1000</f>
         <v>92.7045</v>
       </c>
-      <c r="O21" s="42" t="n">
+      <c r="O21" s="43" t="n">
         <f aca="false">H21*G21</f>
         <v>547.2696</v>
       </c>
-      <c r="P21" s="42" t="n">
+      <c r="P21" s="43" t="n">
         <f aca="false">J21*N21</f>
         <v>83.6325</v>
       </c>
-      <c r="Q21" s="43" t="n">
+      <c r="Q21" s="44" t="n">
         <f aca="false">P21/O21*100</f>
         <v>15.2817733709309</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="38" t="n">
+      <c r="E22" s="39" t="n">
         <v>13</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="38" t="n">
+      <c r="G22" s="39" t="n">
         <v>489.25</v>
       </c>
-      <c r="H22" s="40" t="n">
+      <c r="H22" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="41" t="e">
+      <c r="I22" s="42" t="e">
         <f aca="false">$C$12/F22</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J22" s="41" t="e">
+      <c r="J22" s="42" t="e">
         <f aca="false">I22/$C$11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K22" s="42" t="e">
+      <c r="K22" s="43" t="e">
         <f aca="false">J22*(1/(2*PI()))*60</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L22" s="41" t="n">
+      <c r="L22" s="42" t="n">
         <f aca="false">E22*$C$13</f>
         <v>0.546</v>
       </c>
-      <c r="M22" s="41" t="n">
+      <c r="M22" s="42" t="n">
         <f aca="false">L22*9.81</f>
         <v>5.35626</v>
       </c>
-      <c r="N22" s="41" t="n">
+      <c r="N22" s="42" t="n">
         <f aca="false">M22*$C$11*1000</f>
         <v>100.429875</v>
       </c>
-      <c r="O22" s="42" t="n">
+      <c r="O22" s="43" t="n">
         <f aca="false">H22*G22</f>
         <v>0</v>
       </c>
-      <c r="P22" s="42" t="e">
+      <c r="P22" s="43" t="e">
         <f aca="false">J22*N22</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q22" s="43" t="e">
+      <c r="Q22" s="44" t="e">
         <f aca="false">P22/O22*100</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E23" s="43"/>
-      <c r="K23" s="4" t="s">
+      <c r="E23" s="44"/>
+      <c r="K23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="W23" s="4" t="s">
+      <c r="W23" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="S24" s="6" t="s">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="S24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="W24" s="6" t="s">
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="W24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="X24" s="6"/>
-      <c r="Z24" s="12" t="s">
+      <c r="X24" s="7"/>
+      <c r="Z24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
-      <c r="AE24" s="12"/>
-      <c r="AK24" s="12" t="s">
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
+      <c r="AK24" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AL24" s="12"/>
-      <c r="AM24" s="12"/>
-      <c r="AN24" s="12"/>
-      <c r="AO24" s="12"/>
-      <c r="AP24" s="12"/>
-      <c r="AS24" s="12" t="s">
+      <c r="AL24" s="13"/>
+      <c r="AM24" s="13"/>
+      <c r="AN24" s="13"/>
+      <c r="AO24" s="13"/>
+      <c r="AP24" s="13"/>
+      <c r="AS24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AT24" s="12"/>
-      <c r="AU24" s="12"/>
-      <c r="AV24" s="12"/>
-      <c r="AW24" s="12"/>
-      <c r="AX24" s="12"/>
+      <c r="AT24" s="13"/>
+      <c r="AU24" s="13"/>
+      <c r="AV24" s="13"/>
+      <c r="AW24" s="13"/>
+      <c r="AX24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N25" s="8" t="s">
+      <c r="N25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O25" s="7" t="s">
+      <c r="O25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="P25" s="7" t="s">
+      <c r="P25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q25" s="7" t="s">
+      <c r="Q25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="S25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="T25" s="10" t="s">
+      <c r="T25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="U25" s="11" t="s">
+      <c r="U25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="W25" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="X25" s="11" t="s">
+      <c r="X25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="12"/>
-      <c r="AC25" s="12"/>
-      <c r="AD25" s="12"/>
-      <c r="AE25" s="12"/>
-      <c r="AK25" s="12"/>
-      <c r="AL25" s="12"/>
-      <c r="AM25" s="12"/>
-      <c r="AN25" s="12"/>
-      <c r="AO25" s="12"/>
-      <c r="AP25" s="12"/>
-      <c r="AS25" s="12"/>
-      <c r="AT25" s="12"/>
-      <c r="AU25" s="12"/>
-      <c r="AV25" s="12"/>
-      <c r="AW25" s="12"/>
-      <c r="AX25" s="12"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AK25" s="13"/>
+      <c r="AL25" s="13"/>
+      <c r="AM25" s="13"/>
+      <c r="AN25" s="13"/>
+      <c r="AO25" s="13"/>
+      <c r="AP25" s="13"/>
+      <c r="AS25" s="13"/>
+      <c r="AT25" s="13"/>
+      <c r="AU25" s="13"/>
+      <c r="AV25" s="13"/>
+      <c r="AW25" s="13"/>
+      <c r="AX25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E26" s="13" t="n">
+      <c r="E26" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="14" t="n">
+      <c r="F26" s="15" t="n">
         <v>3.049</v>
       </c>
-      <c r="G26" s="13" t="n">
+      <c r="G26" s="14" t="n">
         <v>125.61</v>
       </c>
-      <c r="H26" s="15" t="n">
+      <c r="H26" s="16" t="n">
         <v>3.72</v>
       </c>
-      <c r="I26" s="16" t="n">
+      <c r="I26" s="17" t="n">
         <f aca="false">$C$12/F26</f>
         <v>0.193506067563135</v>
       </c>
-      <c r="J26" s="16" t="n">
+      <c r="J26" s="17" t="n">
         <f aca="false">I26/$C$11</f>
         <v>10.3203236033672</v>
       </c>
-      <c r="K26" s="17" t="n">
+      <c r="K26" s="18" t="n">
         <f aca="false">J26*(1/(2*PI()))*60</f>
         <v>98.5518309470313</v>
       </c>
-      <c r="L26" s="18" t="n">
+      <c r="L26" s="19" t="n">
         <f aca="false">E26*$C$13</f>
         <v>0</v>
       </c>
-      <c r="M26" s="44" t="n">
+      <c r="M26" s="45" t="n">
         <f aca="false">L26*9.81</f>
         <v>0</v>
       </c>
-      <c r="N26" s="11" t="n">
+      <c r="N26" s="12" t="n">
         <f aca="false">M26*$C$11*1000</f>
         <v>0</v>
       </c>
-      <c r="O26" s="19" t="n">
+      <c r="O26" s="20" t="n">
         <f aca="false">H26*G26</f>
         <v>467.2692</v>
       </c>
-      <c r="P26" s="17" t="n">
+      <c r="P26" s="18" t="n">
         <f aca="false">J26*N26</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="10" t="n">
+      <c r="Q26" s="11" t="n">
         <f aca="false">P26/O26*100</f>
         <v>0</v>
       </c>
-      <c r="S26" s="20" t="n">
+      <c r="S26" s="21" t="n">
         <v>20</v>
       </c>
-      <c r="T26" s="21" t="n">
+      <c r="T26" s="22" t="n">
         <v>21.241</v>
       </c>
-      <c r="U26" s="11" t="n">
+      <c r="U26" s="12" t="n">
         <f aca="false">(($C$12/T26)/$C$11)/(2*3.141)*60</f>
         <v>14.149109218398</v>
       </c>
-      <c r="W26" s="9"/>
-      <c r="X26" s="11"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
-      <c r="AE26" s="12"/>
-      <c r="AK26" s="12"/>
-      <c r="AL26" s="12"/>
-      <c r="AM26" s="12"/>
-      <c r="AN26" s="12"/>
-      <c r="AO26" s="12"/>
-      <c r="AP26" s="12"/>
-      <c r="AS26" s="12"/>
-      <c r="AT26" s="12"/>
-      <c r="AU26" s="12"/>
-      <c r="AV26" s="12"/>
-      <c r="AW26" s="12"/>
-      <c r="AX26" s="12"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="12"/>
+      <c r="Z26" s="13"/>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13"/>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="13"/>
+      <c r="AE26" s="13"/>
+      <c r="AK26" s="13"/>
+      <c r="AL26" s="13"/>
+      <c r="AM26" s="13"/>
+      <c r="AN26" s="13"/>
+      <c r="AO26" s="13"/>
+      <c r="AP26" s="13"/>
+      <c r="AS26" s="13"/>
+      <c r="AT26" s="13"/>
+      <c r="AU26" s="13"/>
+      <c r="AV26" s="13"/>
+      <c r="AW26" s="13"/>
+      <c r="AX26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="13" t="n">
+      <c r="E27" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="14" t="n">
+      <c r="F27" s="15" t="n">
         <v>3.409</v>
       </c>
-      <c r="G27" s="13" t="n">
+      <c r="G27" s="14" t="n">
         <v>117.79</v>
       </c>
-      <c r="H27" s="23" t="n">
+      <c r="H27" s="24" t="n">
         <v>3.8</v>
       </c>
-      <c r="I27" s="16" t="n">
+      <c r="I27" s="17" t="n">
         <f aca="false">$C$12/F27</f>
         <v>0.173071281900851</v>
       </c>
-      <c r="J27" s="16" t="n">
+      <c r="J27" s="17" t="n">
         <f aca="false">I27/$C$11</f>
         <v>9.23046836804537</v>
       </c>
-      <c r="K27" s="17" t="n">
+      <c r="K27" s="18" t="n">
         <f aca="false">J27*(1/(2*PI()))*60</f>
         <v>88.1444800696681</v>
       </c>
-      <c r="L27" s="18" t="n">
+      <c r="L27" s="19" t="n">
         <f aca="false">E27*$C$13</f>
         <v>0.042</v>
       </c>
-      <c r="M27" s="18" t="n">
+      <c r="M27" s="19" t="n">
         <f aca="false">L27*9.81</f>
         <v>0.41202</v>
       </c>
-      <c r="N27" s="16" t="n">
+      <c r="N27" s="17" t="n">
         <f aca="false">M27*$C$11*1000</f>
         <v>7.725375</v>
       </c>
-      <c r="O27" s="19" t="n">
+      <c r="O27" s="20" t="n">
         <f aca="false">H27*G27</f>
         <v>447.602</v>
       </c>
-      <c r="P27" s="17" t="n">
+      <c r="P27" s="18" t="n">
         <f aca="false">J27*N27</f>
         <v>71.3088295687885</v>
       </c>
-      <c r="Q27" s="10" t="n">
+      <c r="Q27" s="11" t="n">
         <f aca="false">P27/O27*100</f>
         <v>15.9313027128539</v>
       </c>
-      <c r="S27" s="20" t="n">
+      <c r="S27" s="21" t="n">
         <v>40</v>
       </c>
-      <c r="T27" s="21" t="n">
+      <c r="T27" s="22" t="n">
         <v>7.928</v>
       </c>
-      <c r="U27" s="11" t="n">
+      <c r="U27" s="12" t="n">
         <f aca="false">(($C$12/T27)/$C$11)/(2*3.141)*60</f>
         <v>37.9088331115024</v>
       </c>
-      <c r="W27" s="22" t="n">
+      <c r="W27" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="X27" s="15" t="n">
+      <c r="X27" s="16" t="n">
         <v>5.989</v>
       </c>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="12"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
-      <c r="AE27" s="12"/>
-      <c r="AK27" s="12"/>
-      <c r="AL27" s="12"/>
-      <c r="AM27" s="12"/>
-      <c r="AN27" s="12"/>
-      <c r="AO27" s="12"/>
-      <c r="AP27" s="12"/>
-      <c r="AS27" s="12"/>
-      <c r="AT27" s="12"/>
-      <c r="AU27" s="12"/>
-      <c r="AV27" s="12"/>
-      <c r="AW27" s="12"/>
-      <c r="AX27" s="12"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="13"/>
+      <c r="AK27" s="13"/>
+      <c r="AL27" s="13"/>
+      <c r="AM27" s="13"/>
+      <c r="AN27" s="13"/>
+      <c r="AO27" s="13"/>
+      <c r="AP27" s="13"/>
+      <c r="AS27" s="13"/>
+      <c r="AT27" s="13"/>
+      <c r="AU27" s="13"/>
+      <c r="AV27" s="13"/>
+      <c r="AW27" s="13"/>
+      <c r="AX27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="13" t="n">
+      <c r="E28" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F28" s="14" t="n">
+      <c r="F28" s="15" t="n">
         <v>3.845</v>
       </c>
-      <c r="G28" s="13" t="n">
+      <c r="G28" s="14" t="n">
         <v>159.82</v>
       </c>
-      <c r="H28" s="23" t="n">
+      <c r="H28" s="24" t="n">
         <v>3.36</v>
       </c>
-      <c r="I28" s="16" t="n">
+      <c r="I28" s="17" t="n">
         <f aca="false">$C$12/F28</f>
         <v>0.153446033810143</v>
       </c>
-      <c r="J28" s="16" t="n">
+      <c r="J28" s="17" t="n">
         <f aca="false">I28/$C$11</f>
         <v>8.18378846987429</v>
       </c>
-      <c r="K28" s="17" t="n">
+      <c r="K28" s="18" t="n">
         <f aca="false">J28*(1/(2*PI()))*60</f>
         <v>78.1494232919372</v>
       </c>
-      <c r="L28" s="18" t="n">
+      <c r="L28" s="19" t="n">
         <f aca="false">E28*$C$13</f>
         <v>0.084</v>
       </c>
-      <c r="M28" s="18" t="n">
+      <c r="M28" s="19" t="n">
         <f aca="false">L28*9.81</f>
         <v>0.82404</v>
       </c>
-      <c r="N28" s="16" t="n">
+      <c r="N28" s="17" t="n">
         <f aca="false">M28*$C$11*1000</f>
         <v>15.45075</v>
       </c>
-      <c r="O28" s="19" t="n">
+      <c r="O28" s="20" t="n">
         <f aca="false">H28*G28</f>
         <v>536.9952</v>
       </c>
-      <c r="P28" s="17" t="n">
+      <c r="P28" s="18" t="n">
         <f aca="false">J28*N28</f>
         <v>126.44566970091</v>
       </c>
-      <c r="Q28" s="10" t="n">
+      <c r="Q28" s="11" t="n">
         <f aca="false">P28/O28*100</f>
         <v>23.5468901213475</v>
       </c>
-      <c r="S28" s="24" t="n">
+      <c r="S28" s="25" t="n">
         <v>60</v>
       </c>
-      <c r="T28" s="25" t="n">
+      <c r="T28" s="26" t="n">
         <v>5.511</v>
       </c>
-      <c r="U28" s="16" t="n">
+      <c r="U28" s="17" t="n">
         <f aca="false">(($C$12/T28)/$C$11)/(2*3.141)*60</f>
         <v>54.5347902210109</v>
       </c>
-      <c r="W28" s="9" t="n">
+      <c r="W28" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="X28" s="23" t="n">
+      <c r="X28" s="24" t="n">
         <v>5.663</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="13" t="n">
+      <c r="E29" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F29" s="14" t="n">
+      <c r="F29" s="15" t="n">
         <v>4.519</v>
       </c>
-      <c r="G29" s="13" t="n">
+      <c r="G29" s="14" t="n">
         <v>188.66</v>
       </c>
-      <c r="H29" s="23" t="n">
+      <c r="H29" s="24" t="n">
         <v>3.06</v>
       </c>
-      <c r="I29" s="16" t="n">
+      <c r="I29" s="17" t="n">
         <f aca="false">$C$12/F29</f>
         <v>0.130559858375747</v>
       </c>
-      <c r="J29" s="16" t="n">
+      <c r="J29" s="17" t="n">
         <f aca="false">I29/$C$11</f>
         <v>6.9631924467065</v>
       </c>
-      <c r="K29" s="17" t="n">
+      <c r="K29" s="18" t="n">
         <f aca="false">J29*(1/(2*PI()))*60</f>
         <v>66.4935898556093</v>
       </c>
-      <c r="L29" s="18" t="n">
+      <c r="L29" s="19" t="n">
         <f aca="false">E29*$C$13</f>
         <v>0.126</v>
       </c>
-      <c r="M29" s="18" t="n">
+      <c r="M29" s="19" t="n">
         <f aca="false">L29*9.81</f>
         <v>1.23606</v>
       </c>
-      <c r="N29" s="16" t="n">
+      <c r="N29" s="17" t="n">
         <f aca="false">M29*$C$11*1000</f>
         <v>23.176125</v>
       </c>
-      <c r="O29" s="19" t="n">
+      <c r="O29" s="20" t="n">
         <f aca="false">H29*G29</f>
         <v>577.2996</v>
       </c>
-      <c r="P29" s="17" t="n">
+      <c r="P29" s="18" t="n">
         <f aca="false">J29*N29</f>
         <v>161.379818543926</v>
       </c>
-      <c r="Q29" s="10" t="n">
+      <c r="Q29" s="11" t="n">
         <f aca="false">P29/O29*100</f>
         <v>27.9542578141273</v>
       </c>
-      <c r="S29" s="24" t="n">
+      <c r="S29" s="25" t="n">
         <v>80</v>
       </c>
-      <c r="T29" s="25" t="n">
+      <c r="T29" s="26" t="n">
         <v>4.573</v>
       </c>
-      <c r="U29" s="16" t="n">
+      <c r="U29" s="17" t="n">
         <f aca="false">(($C$12/T29)/$C$11)/(2*3.141)*60</f>
         <v>65.7208022978332</v>
       </c>
-      <c r="W29" s="9" t="n">
+      <c r="W29" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="X29" s="23" t="n">
+      <c r="X29" s="24" t="n">
         <v>5.77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="13" t="n">
+      <c r="E30" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F30" s="14" t="n">
+      <c r="F30" s="15" t="n">
         <v>5.393</v>
       </c>
-      <c r="G30" s="13" t="n">
+      <c r="G30" s="14" t="n">
         <v>214.08</v>
       </c>
-      <c r="H30" s="23" t="n">
+      <c r="H30" s="24" t="n">
         <v>2.81</v>
       </c>
-      <c r="I30" s="16" t="n">
+      <c r="I30" s="17" t="n">
         <f aca="false">$C$12/F30</f>
         <v>0.1094010754682</v>
       </c>
-      <c r="J30" s="16" t="n">
+      <c r="J30" s="17" t="n">
         <f aca="false">I30/$C$11</f>
         <v>5.83472402497064</v>
       </c>
-      <c r="K30" s="17" t="n">
+      <c r="K30" s="18" t="n">
         <f aca="false">J30*(1/(2*PI()))*60</f>
         <v>55.717510209067</v>
       </c>
-      <c r="L30" s="18" t="n">
+      <c r="L30" s="19" t="n">
         <f aca="false">E30*$C$13</f>
         <v>0.168</v>
       </c>
-      <c r="M30" s="18" t="n">
+      <c r="M30" s="19" t="n">
         <f aca="false">L30*9.81</f>
         <v>1.64808</v>
       </c>
-      <c r="N30" s="16" t="n">
+      <c r="N30" s="17" t="n">
         <f aca="false">M30*$C$11*1000</f>
         <v>30.9015</v>
       </c>
-      <c r="O30" s="19" t="n">
+      <c r="O30" s="20" t="n">
         <f aca="false">H30*G30</f>
         <v>601.5648</v>
       </c>
-      <c r="P30" s="17" t="n">
+      <c r="P30" s="18" t="n">
         <f aca="false">J30*N30</f>
         <v>180.30172445763</v>
       </c>
-      <c r="Q30" s="10" t="n">
+      <c r="Q30" s="11" t="n">
         <f aca="false">P30/O30*100</f>
         <v>29.9721201203312</v>
       </c>
-      <c r="S30" s="29" t="n">
+      <c r="S30" s="30" t="n">
         <v>100</v>
       </c>
-      <c r="T30" s="30" t="n">
+      <c r="T30" s="31" t="n">
         <v>3.78</v>
       </c>
-      <c r="U30" s="31" t="n">
+      <c r="U30" s="32" t="n">
         <f aca="false">(($C$12/T30)/$C$11)/(2*3.141)*60</f>
         <v>79.5082616158707</v>
       </c>
-      <c r="W30" s="9" t="n">
+      <c r="W30" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="X30" s="23" t="n">
+      <c r="X30" s="24" t="n">
         <v>5.823</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="13" t="n">
+      <c r="E31" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F31" s="14" t="n">
+      <c r="F31" s="15" t="n">
         <v>6.565</v>
       </c>
-      <c r="G31" s="13" t="n">
+      <c r="G31" s="14" t="n">
         <v>243.4</v>
       </c>
-      <c r="H31" s="23" t="n">
+      <c r="H31" s="24" t="n">
         <v>2.49</v>
       </c>
-      <c r="I31" s="16" t="n">
+      <c r="I31" s="17" t="n">
         <f aca="false">$C$12/F31</f>
         <v>0.0898705255140899</v>
       </c>
-      <c r="J31" s="16" t="n">
+      <c r="J31" s="17" t="n">
         <f aca="false">I31/$C$11</f>
         <v>4.79309469408479</v>
       </c>
-      <c r="K31" s="17" t="n">
+      <c r="K31" s="18" t="n">
         <f aca="false">J31*(1/(2*PI()))*60</f>
         <v>45.7706827962679</v>
       </c>
-      <c r="L31" s="18" t="n">
+      <c r="L31" s="19" t="n">
         <f aca="false">E31*$C$13</f>
         <v>0.21</v>
       </c>
-      <c r="M31" s="18" t="n">
+      <c r="M31" s="19" t="n">
         <f aca="false">L31*9.81</f>
         <v>2.0601</v>
       </c>
-      <c r="N31" s="16" t="n">
+      <c r="N31" s="17" t="n">
         <f aca="false">M31*$C$11*1000</f>
         <v>38.626875</v>
       </c>
-      <c r="O31" s="19" t="n">
+      <c r="O31" s="20" t="n">
         <f aca="false">H31*G31</f>
         <v>606.066</v>
       </c>
-      <c r="P31" s="17" t="n">
+      <c r="P31" s="18" t="n">
         <f aca="false">J31*N31</f>
         <v>185.142269611577</v>
       </c>
-      <c r="Q31" s="10" t="n">
+      <c r="Q31" s="11" t="n">
         <f aca="false">P31/O31*100</f>
         <v>30.5482026069069</v>
       </c>
-      <c r="W31" s="9" t="n">
+      <c r="W31" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="X31" s="23" t="n">
+      <c r="X31" s="24" t="n">
         <v>5.952</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="13" t="n">
+      <c r="E32" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F32" s="14" t="n">
+      <c r="F32" s="15" t="n">
         <v>7.68</v>
       </c>
-      <c r="G32" s="13" t="n">
+      <c r="G32" s="14" t="n">
         <v>273.22</v>
       </c>
-      <c r="H32" s="23" t="n">
+      <c r="H32" s="24" t="n">
         <v>2.18</v>
       </c>
-      <c r="I32" s="16" t="n">
+      <c r="I32" s="17" t="n">
         <f aca="false">$C$12/F32</f>
         <v>0.0768229166666667</v>
       </c>
-      <c r="J32" s="16" t="n">
+      <c r="J32" s="17" t="n">
         <f aca="false">I32/$C$11</f>
         <v>4.09722222222222</v>
       </c>
-      <c r="K32" s="17" t="n">
+      <c r="K32" s="18" t="n">
         <f aca="false">J32*(1/(2*PI()))*60</f>
         <v>39.1255901767576</v>
       </c>
-      <c r="L32" s="18" t="n">
+      <c r="L32" s="19" t="n">
         <f aca="false">E32*$C$13</f>
         <v>0.252</v>
       </c>
-      <c r="M32" s="18" t="n">
+      <c r="M32" s="19" t="n">
         <f aca="false">L32*9.81</f>
         <v>2.47212</v>
       </c>
-      <c r="N32" s="16" t="n">
+      <c r="N32" s="17" t="n">
         <f aca="false">M32*$C$11*1000</f>
         <v>46.35225</v>
       </c>
-      <c r="O32" s="19" t="n">
+      <c r="O32" s="20" t="n">
         <f aca="false">H32*G32</f>
         <v>595.6196</v>
       </c>
-      <c r="P32" s="17" t="n">
+      <c r="P32" s="18" t="n">
         <f aca="false">J32*N32</f>
         <v>189.91546875</v>
       </c>
-      <c r="Q32" s="10" t="n">
+      <c r="Q32" s="11" t="n">
         <f aca="false">P32/O32*100</f>
         <v>31.8853625283654</v>
       </c>
-      <c r="W32" s="9" t="n">
+      <c r="W32" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="X32" s="23" t="n">
+      <c r="X32" s="24" t="n">
         <v>5.735</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="13" t="n">
+      <c r="E33" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F33" s="14" t="n">
+      <c r="F33" s="15" t="n">
         <v>10.639</v>
       </c>
-      <c r="G33" s="13" t="n">
+      <c r="G33" s="14" t="n">
         <v>281.52</v>
       </c>
-      <c r="H33" s="23" t="n">
+      <c r="H33" s="24" t="n">
         <v>2.11</v>
       </c>
-      <c r="I33" s="16" t="n">
+      <c r="I33" s="17" t="n">
         <f aca="false">$C$12/F33</f>
         <v>0.0554563398815678</v>
       </c>
-      <c r="J33" s="16" t="n">
+      <c r="J33" s="17" t="n">
         <f aca="false">I33/$C$11</f>
         <v>2.95767146035028</v>
       </c>
-      <c r="K33" s="17" t="n">
+      <c r="K33" s="18" t="n">
         <f aca="false">J33*(1/(2*PI()))*60</f>
         <v>28.2436819773943</v>
       </c>
-      <c r="L33" s="18" t="n">
+      <c r="L33" s="19" t="n">
         <f aca="false">E33*$C$13</f>
         <v>0.294</v>
       </c>
-      <c r="M33" s="18" t="n">
+      <c r="M33" s="19" t="n">
         <f aca="false">L33*9.81</f>
         <v>2.88414</v>
       </c>
-      <c r="N33" s="16" t="n">
+      <c r="N33" s="17" t="n">
         <f aca="false">M33*$C$11*1000</f>
         <v>54.077625</v>
       </c>
-      <c r="O33" s="19" t="n">
+      <c r="O33" s="20" t="n">
         <f aca="false">H33*G33</f>
         <v>594.0072</v>
       </c>
-      <c r="P33" s="17" t="n">
+      <c r="P33" s="18" t="n">
         <f aca="false">J33*N33</f>
         <v>159.943848106025</v>
       </c>
-      <c r="Q33" s="10" t="n">
+      <c r="Q33" s="11" t="n">
         <f aca="false">P33/O33*100</f>
         <v>26.926247376467</v>
       </c>
-      <c r="W33" s="9" t="n">
+      <c r="W33" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="X33" s="23" t="n">
+      <c r="X33" s="24" t="n">
         <v>5.661</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="13" t="n">
+      <c r="E34" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F34" s="14" t="n">
+      <c r="F34" s="15" t="n">
         <v>16.202</v>
       </c>
-      <c r="G34" s="13" t="n">
+      <c r="G34" s="14" t="n">
         <v>332.36</v>
       </c>
-      <c r="H34" s="23" t="n">
+      <c r="H34" s="24" t="n">
         <v>1.59</v>
       </c>
-      <c r="I34" s="16" t="n">
+      <c r="I34" s="17" t="n">
         <f aca="false">$C$12/F34</f>
         <v>0.0364152573756326</v>
       </c>
-      <c r="J34" s="16" t="n">
+      <c r="J34" s="17" t="n">
         <f aca="false">I34/$C$11</f>
         <v>1.94214706003374</v>
       </c>
-      <c r="K34" s="17" t="n">
+      <c r="K34" s="18" t="n">
         <f aca="false">J34*(1/(2*PI()))*60</f>
         <v>18.5461382889457</v>
       </c>
-      <c r="L34" s="18" t="n">
+      <c r="L34" s="19" t="n">
         <f aca="false">E34*$C$13</f>
         <v>0.336</v>
       </c>
-      <c r="M34" s="18" t="n">
+      <c r="M34" s="19" t="n">
         <f aca="false">L34*9.81</f>
         <v>3.29616</v>
       </c>
-      <c r="N34" s="16" t="n">
+      <c r="N34" s="17" t="n">
         <f aca="false">M34*$C$11*1000</f>
         <v>61.803</v>
       </c>
-      <c r="O34" s="19" t="n">
+      <c r="O34" s="20" t="n">
         <f aca="false">H34*G34</f>
         <v>528.4524</v>
       </c>
-      <c r="P34" s="17" t="n">
+      <c r="P34" s="18" t="n">
         <f aca="false">J34*N34</f>
         <v>120.030514751265</v>
       </c>
-      <c r="Q34" s="10" t="n">
+      <c r="Q34" s="11" t="n">
         <f aca="false">P34/O34*100</f>
         <v>22.7135906188079</v>
       </c>
-      <c r="W34" s="9" t="n">
+      <c r="W34" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="X34" s="23" t="n">
+      <c r="X34" s="24" t="n">
         <v>5.57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="33" t="n">
+      <c r="E35" s="34" t="n">
         <v>9</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G35" s="33" t="n">
+      <c r="G35" s="34" t="n">
         <v>488.27</v>
       </c>
-      <c r="H35" s="28" t="n">
+      <c r="H35" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="31" t="e">
+      <c r="I35" s="32" t="e">
         <f aca="false">$C$12/F35</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J35" s="31" t="e">
+      <c r="J35" s="32" t="e">
         <f aca="false">I35/$C$11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="35" t="e">
+      <c r="K35" s="36" t="e">
         <f aca="false">J35*(1/(2*PI()))*60</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L35" s="36" t="n">
+      <c r="L35" s="37" t="n">
         <f aca="false">E35*$C$13</f>
         <v>0.378</v>
       </c>
-      <c r="M35" s="36" t="n">
+      <c r="M35" s="37" t="n">
         <f aca="false">L35*9.81</f>
         <v>3.70818</v>
       </c>
-      <c r="N35" s="31" t="n">
+      <c r="N35" s="32" t="n">
         <f aca="false">M35*$C$11*1000</f>
         <v>69.528375</v>
       </c>
-      <c r="O35" s="35" t="n">
+      <c r="O35" s="36" t="n">
         <f aca="false">H35*G35</f>
         <v>0</v>
       </c>
-      <c r="P35" s="35" t="e">
+      <c r="P35" s="36" t="e">
         <f aca="false">J35*N35</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q35" s="37" t="e">
+      <c r="Q35" s="38" t="e">
         <f aca="false">P35/O35*100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="W35" s="9" t="n">
+      <c r="W35" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="X35" s="23" t="n">
+      <c r="X35" s="24" t="n">
         <v>5.807</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W36" s="32" t="n">
+      <c r="W36" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="X36" s="28" t="n">
+      <c r="X36" s="29" t="n">
         <v>5.698</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated speed vs torque graphs
</commit_message>
<xml_diff>
--- a/Lab1/lab1Results.xlsx
+++ b/Lab1/lab1Results.xlsx
@@ -1368,8 +1368,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61485303"/>
-        <c:axId val="97403365"/>
+        <c:axId val="45659995"/>
+        <c:axId val="80888307"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1552,13 +1552,14 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96659038"/>
-        <c:axId val="66225298"/>
+        <c:axId val="16103174"/>
+        <c:axId val="43524638"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61485303"/>
+        <c:axId val="45659995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1632,12 +1633,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97403365"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="80888307"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97403365"/>
+        <c:axId val="80888307"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,12 +1714,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61485303"/>
+        <c:crossAx val="45659995"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96659038"/>
+        <c:axId val="16103174"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,11 +1751,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66225298"/>
+        <c:crossAx val="43524638"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66225298"/>
+        <c:axId val="43524638"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1821,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96659038"/>
+        <c:crossAx val="16103174"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2070,8 +2071,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18331283"/>
-        <c:axId val="47517182"/>
+        <c:axId val="13899071"/>
+        <c:axId val="29624151"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2230,13 +2231,14 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="95324960"/>
-        <c:axId val="42435816"/>
+        <c:axId val="43605153"/>
+        <c:axId val="30375538"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18331283"/>
+        <c:axId val="13899071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2310,12 +2312,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47517182"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="29624151"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47517182"/>
+        <c:axId val="29624151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,12 +2393,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18331283"/>
+        <c:crossAx val="13899071"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95324960"/>
+        <c:axId val="43605153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,11 +2430,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42435816"/>
+        <c:crossAx val="30375538"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42435816"/>
+        <c:axId val="30375538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,7 +2500,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95324960"/>
+        <c:crossAx val="43605153"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2773,8 +2775,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52434138"/>
-        <c:axId val="51040387"/>
+        <c:axId val="70011912"/>
+        <c:axId val="72473016"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2957,11 +2959,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52373319"/>
-        <c:axId val="14943033"/>
+        <c:axId val="14619835"/>
+        <c:axId val="85510433"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52434138"/>
+        <c:axId val="70011912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,12 +3039,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51040387"/>
+        <c:crossAx val="72473016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51040387"/>
+        <c:axId val="72473016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3118,12 +3120,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52434138"/>
+        <c:crossAx val="70011912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52373319"/>
+        <c:axId val="14619835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3155,11 +3157,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14943033"/>
+        <c:crossAx val="85510433"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14943033"/>
+        <c:axId val="85510433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,7 +3227,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52373319"/>
+        <c:crossAx val="14619835"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3476,8 +3478,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97674353"/>
-        <c:axId val="91657236"/>
+        <c:axId val="91500227"/>
+        <c:axId val="15997417"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3660,11 +3662,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18722890"/>
-        <c:axId val="27758769"/>
+        <c:axId val="43462703"/>
+        <c:axId val="63477098"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97674353"/>
+        <c:axId val="91500227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3740,12 +3742,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91657236"/>
+        <c:crossAx val="15997417"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91657236"/>
+        <c:axId val="15997417"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3821,12 +3823,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97674353"/>
+        <c:crossAx val="91500227"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18722890"/>
+        <c:axId val="43462703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3858,11 +3860,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27758769"/>
+        <c:crossAx val="63477098"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27758769"/>
+        <c:axId val="63477098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3928,7 +3930,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18722890"/>
+        <c:crossAx val="43462703"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4030,11 +4032,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$8</c:f>
+              <c:f>Sheet1!$U$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PWM setting (%)</c:v>
+                  <c:v>w (rpm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4152,11 +4154,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34948244"/>
-        <c:axId val="58832852"/>
+        <c:axId val="99208466"/>
+        <c:axId val="98371595"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34948244"/>
+        <c:axId val="99208466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4233,12 +4235,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58832852"/>
+        <c:crossAx val="98371595"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58832852"/>
+        <c:axId val="98371595"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -4315,7 +4317,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34948244"/>
+        <c:crossAx val="99208466"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4416,11 +4418,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$25</c:f>
+              <c:f>Sheet1!$U$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PWM setting (%)</c:v>
+                  <c:v>w (rpm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4538,11 +4540,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="99563074"/>
-        <c:axId val="35435526"/>
+        <c:axId val="31045105"/>
+        <c:axId val="68292901"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99563074"/>
+        <c:axId val="31045105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4619,12 +4621,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35435526"/>
+        <c:crossAx val="68292901"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35435526"/>
+        <c:axId val="68292901"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -4701,7 +4703,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99563074"/>
+        <c:crossAx val="31045105"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4750,7 +4752,6 @@
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -4765,9 +4766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4775,8 +4776,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21888720" y="2030400"/>
-        <a:ext cx="4995000" cy="2816640"/>
+        <a:off x="21888000" y="2030400"/>
+        <a:ext cx="4995000" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4795,9 +4796,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4805,8 +4806,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21890880" y="5456160"/>
-        <a:ext cx="4995000" cy="2816640"/>
+        <a:off x="21890160" y="5456160"/>
+        <a:ext cx="4995000" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4825,9 +4826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>234720</xdr:colOff>
+      <xdr:colOff>234360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4835,8 +4836,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28150920" y="2079360"/>
-        <a:ext cx="4995360" cy="2816640"/>
+        <a:off x="28150200" y="2079360"/>
+        <a:ext cx="4995000" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4855,9 +4856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>118440</xdr:colOff>
+      <xdr:colOff>118080</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4865,8 +4866,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28034640" y="5262840"/>
-        <a:ext cx="4995360" cy="2816640"/>
+        <a:off x="28033920" y="5262840"/>
+        <a:ext cx="4995000" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4885,9 +4886,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>43200</xdr:colOff>
+      <xdr:colOff>42840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>178560</xdr:rowOff>
+      <xdr:rowOff>178200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4895,8 +4896,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33463080" y="2091240"/>
-        <a:ext cx="4995000" cy="2816640"/>
+        <a:off x="33462360" y="2091240"/>
+        <a:ext cx="4994640" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4915,9 +4916,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4925,8 +4926,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33496200" y="5243040"/>
-        <a:ext cx="4995000" cy="2816640"/>
+        <a:off x="33495480" y="5243040"/>
+        <a:ext cx="4994640" cy="2816280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4947,8 +4948,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0719948111847795</cdr:x>
-      <cdr:y>0.127667731629393</cdr:y>
+      <cdr:x>0.0719227443067166</cdr:x>
+      <cdr:y>0.127556237218814</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -4962,7 +4963,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="359640" cy="359640"/>
+          <a:ext cx="359280" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4984,8 +4985,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0719948111847795</cdr:x>
-      <cdr:y>0.127667731629393</cdr:y>
+      <cdr:x>0.0719227443067166</cdr:x>
+      <cdr:y>0.127556237218814</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -4999,7 +5000,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="359640" cy="359640"/>
+          <a:ext cx="359280" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5021,8 +5022,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0719896231173885</cdr:x>
-      <cdr:y>0.127667731629393</cdr:y>
+      <cdr:x>0.0719227443067166</cdr:x>
+      <cdr:y>0.127556237218814</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -5036,7 +5037,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="359640" cy="359640"/>
+          <a:ext cx="359280" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5058,8 +5059,8 @@
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.0719896231173885</cdr:x>
-      <cdr:y>0.127667731629393</cdr:y>
+      <cdr:x>0.0719227443067166</cdr:x>
+      <cdr:y>0.127556237218814</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -5073,44 +5074,7 @@
       <cdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="359640" cy="359640"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </cdr:spPr>
-    </cdr:pic>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <cdr:relSizeAnchor>
-    <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.0719948111847795</cdr:x>
-      <cdr:y>0.127667731629393</cdr:y>
-    </cdr:to>
-    <cdr:pic>
-      <cdr:nvPicPr>
-        <cdr:cNvPr id="10" name="" descr=""/>
-        <cdr:cNvPicPr/>
-      </cdr:nvPicPr>
-      <cdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </cdr:blipFill>
-      <cdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="359640" cy="359640"/>
+          <a:ext cx="359280" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5303,8 +5267,8 @@
   </sheetPr>
   <dimension ref="A1:AX36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO6" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BB27" activeCellId="0" sqref="BB27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI14" activeCellId="0" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changed the motor driver sheild to false and added a while loop to freeze the code to wait for the pushbutton
</commit_message>
<xml_diff>
--- a/Lab1/lab1Results.xlsx
+++ b/Lab1/lab1Results.xlsx
@@ -519,7 +519,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t xml:space="preserve">Lab #1: Motor Characterization</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mass per Washer (kg):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Dev:</t>
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
@@ -1368,8 +1374,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45659995"/>
-        <c:axId val="80888307"/>
+        <c:axId val="8889181"/>
+        <c:axId val="22115018"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1552,11 +1558,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16103174"/>
-        <c:axId val="43524638"/>
+        <c:axId val="2900459"/>
+        <c:axId val="5988617"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45659995"/>
+        <c:axId val="8889181"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1633,12 +1639,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80888307"/>
+        <c:crossAx val="22115018"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80888307"/>
+        <c:axId val="22115018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,12 +1720,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45659995"/>
+        <c:crossAx val="8889181"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16103174"/>
+        <c:axId val="2900459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,11 +1757,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43524638"/>
+        <c:crossAx val="5988617"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43524638"/>
+        <c:axId val="5988617"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16103174"/>
+        <c:crossAx val="2900459"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1870,7 +1876,6 @@
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -2071,8 +2076,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13899071"/>
-        <c:axId val="29624151"/>
+        <c:axId val="81900212"/>
+        <c:axId val="45241516"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2231,11 +2236,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="43605153"/>
-        <c:axId val="30375538"/>
+        <c:axId val="41059516"/>
+        <c:axId val="89104407"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13899071"/>
+        <c:axId val="81900212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2312,12 +2317,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29624151"/>
+        <c:crossAx val="45241516"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29624151"/>
+        <c:axId val="45241516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2393,12 +2398,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13899071"/>
+        <c:crossAx val="81900212"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43605153"/>
+        <c:axId val="41059516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,11 +2435,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30375538"/>
+        <c:crossAx val="89104407"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30375538"/>
+        <c:axId val="89104407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2500,7 +2505,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43605153"/>
+        <c:crossAx val="41059516"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2549,7 +2554,6 @@
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -2775,8 +2779,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="70011912"/>
-        <c:axId val="72473016"/>
+        <c:axId val="13845548"/>
+        <c:axId val="1498973"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2959,11 +2963,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="14619835"/>
-        <c:axId val="85510433"/>
+        <c:axId val="41965521"/>
+        <c:axId val="62641083"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70011912"/>
+        <c:axId val="13845548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3039,12 +3043,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72473016"/>
+        <c:crossAx val="1498973"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72473016"/>
+        <c:axId val="1498973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3120,12 +3124,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70011912"/>
+        <c:crossAx val="13845548"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14619835"/>
+        <c:axId val="41965521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3157,11 +3161,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85510433"/>
+        <c:crossAx val="62641083"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85510433"/>
+        <c:axId val="62641083"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3227,7 +3231,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14619835"/>
+        <c:crossAx val="41965521"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3478,8 +3482,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91500227"/>
-        <c:axId val="15997417"/>
+        <c:axId val="20136000"/>
+        <c:axId val="30010937"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3662,11 +3666,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="43462703"/>
-        <c:axId val="63477098"/>
+        <c:axId val="36193230"/>
+        <c:axId val="85107221"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91500227"/>
+        <c:axId val="20136000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,12 +3746,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15997417"/>
+        <c:crossAx val="30010937"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15997417"/>
+        <c:axId val="30010937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,12 +3827,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91500227"/>
+        <c:crossAx val="20136000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43462703"/>
+        <c:axId val="36193230"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3860,11 +3864,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63477098"/>
+        <c:crossAx val="85107221"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63477098"/>
+        <c:axId val="85107221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3930,7 +3934,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43462703"/>
+        <c:crossAx val="36193230"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4154,11 +4158,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="99208466"/>
-        <c:axId val="98371595"/>
+        <c:axId val="44646459"/>
+        <c:axId val="30317132"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99208466"/>
+        <c:axId val="44646459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4235,12 +4239,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98371595"/>
+        <c:crossAx val="30317132"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98371595"/>
+        <c:axId val="30317132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -4317,7 +4321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99208466"/>
+        <c:crossAx val="44646459"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4540,11 +4544,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="31045105"/>
-        <c:axId val="68292901"/>
+        <c:axId val="27358819"/>
+        <c:axId val="60178757"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31045105"/>
+        <c:axId val="27358819"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4621,12 +4625,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68292901"/>
+        <c:crossAx val="60178757"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68292901"/>
+        <c:axId val="60178757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -4703,7 +4707,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31045105"/>
+        <c:crossAx val="27358819"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4802,7 +4806,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2"/>
+        <xdr:cNvPr id="1" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4832,7 +4836,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4862,7 +4866,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 4"/>
+        <xdr:cNvPr id="4" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4892,7 +4896,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4922,7 +4926,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4953,7 +4957,7 @@
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
-        <cdr:cNvPr id="1" name="" descr=""/>
+        <cdr:cNvPr id="3" name="" descr=""/>
         <cdr:cNvPicPr/>
       </cdr:nvPicPr>
       <cdr:blipFill>
@@ -4990,81 +4994,7 @@
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
-        <cdr:cNvPr id="3" name="" descr=""/>
-        <cdr:cNvPicPr/>
-      </cdr:nvPicPr>
-      <cdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </cdr:blipFill>
-      <cdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="359280" cy="359280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </cdr:spPr>
-    </cdr:pic>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <cdr:relSizeAnchor>
-    <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.0719227443067166</cdr:x>
-      <cdr:y>0.127556237218814</cdr:y>
-    </cdr:to>
-    <cdr:pic>
-      <cdr:nvPicPr>
         <cdr:cNvPr id="5" name="" descr=""/>
-        <cdr:cNvPicPr/>
-      </cdr:nvPicPr>
-      <cdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </cdr:blipFill>
-      <cdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="359280" cy="359280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </cdr:spPr>
-    </cdr:pic>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <cdr:relSizeAnchor>
-    <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.0719227443067166</cdr:x>
-      <cdr:y>0.127556237218814</cdr:y>
-    </cdr:to>
-    <cdr:pic>
-      <cdr:nvPicPr>
-        <cdr:cNvPr id="7" name="" descr=""/>
         <cdr:cNvPicPr/>
       </cdr:nvPicPr>
       <cdr:blipFill>
@@ -5265,10 +5195,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX36"/>
+  <dimension ref="A1:AX39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI14" activeCellId="0" sqref="AI14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X40" activeCellId="0" sqref="X40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6201,6 +6131,13 @@
         <f aca="false">P20/O20*100</f>
         <v>26.800638084921</v>
       </c>
+      <c r="W20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <f aca="false">AVERAGE(X9:X18)</f>
+        <v>6.7361</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="39" t="n">
@@ -6251,13 +6188,20 @@
         <f aca="false">P21/O21*100</f>
         <v>15.2817733709309</v>
       </c>
+      <c r="W21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <f aca="false">STDEV(X9:X18)</f>
+        <v>0.113424913978857</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="39" t="n">
         <v>13</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G22" s="39" t="n">
         <v>489.25</v>
@@ -6305,7 +6249,7 @@
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E23" s="44"/>
       <c r="K23" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="W23" s="5" t="s">
         <v>8</v>
@@ -6313,7 +6257,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E24" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -6328,16 +6272,16 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="S24" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
       <c r="W24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="X24" s="7"/>
       <c r="Z24" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
@@ -6345,7 +6289,7 @@
       <c r="AD24" s="13"/>
       <c r="AE24" s="13"/>
       <c r="AK24" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AL24" s="13"/>
       <c r="AM24" s="13"/>
@@ -6353,7 +6297,7 @@
       <c r="AO24" s="13"/>
       <c r="AP24" s="13"/>
       <c r="AS24" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AT24" s="13"/>
       <c r="AU24" s="13"/>
@@ -7026,7 +6970,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G35" s="34" t="n">
         <v>488.27</v>
@@ -7083,6 +7027,24 @@
       </c>
       <c r="X36" s="29" t="n">
         <v>5.698</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X38" s="1" t="n">
+        <f aca="false">AVERAGE(X27:X36)</f>
+        <v>5.7668</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X39" s="1" t="n">
+        <f aca="false">STDEV(X27:X36)</f>
+        <v>0.131190954972767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>